<commit_message>
Add files to another branch
</commit_message>
<xml_diff>
--- a/grades25.xlsx
+++ b/grades25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thebandik/Library/Mobile Documents/com~apple~CloudDocs/General/Work/ВВГУ/GitHub/vvsu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A10006B-8843-484A-ADD0-FC2A41EA1EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708CA714-06B3-1D46-B251-B7E954BA7C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="2300" windowWidth="25600" windowHeight="13900" activeTab="11" xr2:uid="{88B8D92F-FB7A-6344-9111-CF5B0A8ADE6C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{88B8D92F-FB7A-6344-9111-CF5B0A8ADE6C}"/>
   </bookViews>
   <sheets>
     <sheet name="СО-РД-24" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="280">
   <si>
     <t>№</t>
   </si>
@@ -1086,7 +1086,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="41">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1779,11 +1809,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88AA26F2-A649-9345-8698-F18018E0D736}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="142" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1792,16 +1822,15 @@
     <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="6.5" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1832,8 +1861,11 @@
       <c r="J2" s="6">
         <v>45707</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="6">
+        <v>45712</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1864,8 +1896,11 @@
       <c r="J3" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1896,8 +1931,11 @@
       <c r="J4" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1928,8 +1966,11 @@
       <c r="J5" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1960,8 +2001,11 @@
       <c r="J6" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1992,8 +2036,11 @@
       <c r="J7" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2024,8 +2071,11 @@
       <c r="J8" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2056,8 +2106,11 @@
       <c r="J9" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2088,8 +2141,11 @@
       <c r="J10" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2120,8 +2176,11 @@
       <c r="J11" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2152,8 +2211,11 @@
       <c r="J12" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2184,8 +2246,11 @@
       <c r="J13" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2216,8 +2281,11 @@
       <c r="J14" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2248,8 +2316,11 @@
       <c r="J15" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2278,6 +2349,9 @@
         <v>18</v>
       </c>
       <c r="J16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2312,6 +2386,9 @@
       <c r="J17" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="K17" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -2344,6 +2421,9 @@
       <c r="J18" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="K18" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
@@ -2889,24 +2969,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD20 A21 C21:XFD21 A22:B22 D22:XFD22 C23:XFD31 C32:C36 D32:XFD37">
-    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
       <formula>"="</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
       <formula>"+"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="6" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:XFD1048576">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
       <formula>"="</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
       <formula>"+"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2920,14 +3000,14 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView zoomScale="141" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -2945,7 +3025,9 @@
       <c r="C2" s="17">
         <v>45703</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="17">
+        <v>45710</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -2963,7 +3045,9 @@
       <c r="C3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -2981,7 +3065,9 @@
       <c r="C4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -2999,7 +3085,9 @@
       <c r="C5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -3017,7 +3105,9 @@
       <c r="C6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -3035,7 +3125,9 @@
       <c r="C7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -3053,7 +3145,9 @@
       <c r="C8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -3071,7 +3165,9 @@
       <c r="C9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -3089,7 +3185,9 @@
       <c r="C10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -3107,7 +3205,9 @@
       <c r="C11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -3125,7 +3225,9 @@
       <c r="C12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -3143,7 +3245,9 @@
       <c r="C13" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -3161,7 +3265,9 @@
       <c r="C14" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -3179,7 +3285,9 @@
       <c r="C15" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -3197,7 +3305,9 @@
       <c r="C16" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -3215,7 +3325,9 @@
       <c r="C17" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -3233,7 +3345,9 @@
       <c r="C18" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -3251,7 +3365,9 @@
       <c r="C19" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -3269,7 +3385,9 @@
       <c r="C20" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="18" t="s">
+        <v>158</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -3287,7 +3405,9 @@
       <c r="C21" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -3296,7 +3416,446 @@
       <c r="J21" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C21">
+  <conditionalFormatting sqref="C2:D21">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"="</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"+"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F7DBDD-68AD-8D44-B606-30A633915157}">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView zoomScale="156" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>45703</v>
+      </c>
+      <c r="D2" s="6">
+        <v>45710</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:B20">
+    <sortCondition ref="B3:B20"/>
+  </sortState>
+  <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"="</formula>
     </cfRule>
@@ -3308,396 +3867,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F7DBDD-68AD-8D44-B606-30A633915157}">
-  <dimension ref="A1:K20"/>
-  <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="10.83203125" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6">
-        <v>45703</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:B20">
-    <sortCondition ref="B3:B20"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
@@ -3706,8 +3875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A18EEC-3E0A-D549-B97F-97C9D91EEA23}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4122,7 +4291,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:B19">
     <sortCondition ref="B3:B19"/>
   </sortState>
-  <conditionalFormatting sqref="A1:XFD2 A20:XFD1048576 A3:D19 F3:XFD19">
+  <conditionalFormatting sqref="A1:XFD2 A3:D19 F3:XFD19 A20:XFD1048576">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"="</formula>
     </cfRule>
@@ -4140,10 +4309,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C7634E-01C4-A44D-9A81-9E2D73111B54}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView zoomScale="134" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4153,16 +4322,15 @@
     <col min="3" max="3" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="6.5" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="4"/>
+    <col min="9" max="13" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4196,8 +4364,14 @@
       <c r="K2" s="6">
         <v>45706</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="6">
+        <v>45712</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4231,8 +4405,14 @@
       <c r="K3" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4266,8 +4446,14 @@
       <c r="K4" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="3"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4301,8 +4487,14 @@
       <c r="K5" s="3" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="3"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4336,8 +4528,14 @@
       <c r="K6" s="3" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="3"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -4371,8 +4569,14 @@
       <c r="K7" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -4406,8 +4610,14 @@
       <c r="K8" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="3"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -4441,8 +4651,14 @@
       <c r="K9" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="3"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -4476,8 +4692,14 @@
       <c r="K10" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="3"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -4511,8 +4733,14 @@
       <c r="K11" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -4546,8 +4774,14 @@
       <c r="K12" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -4581,8 +4815,14 @@
       <c r="K13" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="3"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4616,8 +4856,14 @@
       <c r="K14" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M14" s="3"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4651,8 +4897,14 @@
       <c r="K15" s="3" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -4686,8 +4938,14 @@
       <c r="K16" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -4721,8 +4979,14 @@
       <c r="K17" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="3"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -4756,8 +5020,14 @@
       <c r="K18" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="3"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -4791,8 +5061,14 @@
       <c r="K19" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="3"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -4826,8 +5102,14 @@
       <c r="K20" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M20" s="3"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -4861,8 +5143,14 @@
       <c r="K21" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M21" s="3"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -4896,8 +5184,14 @@
       <c r="K22" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M22" s="3"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -4931,8 +5225,14 @@
       <c r="K23" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M23" s="3"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -4966,8 +5266,14 @@
       <c r="K24" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M24" s="3"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -5001,8 +5307,14 @@
       <c r="K25" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M25" s="3"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -5036,8 +5348,14 @@
       <c r="K26" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M26" s="3"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -5071,21 +5389,27 @@
       <c r="K27" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M27" s="3"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B29" s="10" t="s">
         <v>105</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:XFD27 A2:F27 A28:XFD1048576">
-    <cfRule type="cellIs" dxfId="31" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
       <formula>"="</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
       <formula>"+"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6023,13 +6347,13 @@
     <sortCondition ref="B2:B21"/>
   </sortState>
   <conditionalFormatting sqref="A1:XFD43 A44 C44:XFD44 A45:XFD1048576">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"="</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"+"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6042,11 +6366,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B95EA0B-B46D-1D4A-BFE5-F97D31298B5D}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView zoomScale="166" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomRight" activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6057,8 +6381,8 @@
     <col min="8" max="9" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="10.83203125" style="4"/>
+    <col min="13" max="15" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -6104,7 +6428,9 @@
       <c r="N1" s="6">
         <v>45708</v>
       </c>
-      <c r="O1" s="3"/>
+      <c r="O1" s="6">
+        <v>45713</v>
+      </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
@@ -6153,7 +6479,9 @@
       <c r="N2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="3"/>
+      <c r="O2" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
@@ -6202,7 +6530,9 @@
       <c r="N3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="3"/>
+      <c r="O3" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
@@ -6251,7 +6581,9 @@
       <c r="N4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="3"/>
+      <c r="O4" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
@@ -6300,7 +6632,9 @@
       <c r="N5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O5" s="3"/>
+      <c r="O5" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
@@ -6349,7 +6683,9 @@
       <c r="N6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="3"/>
+      <c r="O6" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
@@ -6398,7 +6734,9 @@
       <c r="N7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O7" s="3"/>
+      <c r="O7" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
@@ -6447,7 +6785,9 @@
       <c r="N8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O8" s="3"/>
+      <c r="O8" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
@@ -6496,7 +6836,9 @@
       <c r="N9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O9" s="3"/>
+      <c r="O9" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
@@ -6545,7 +6887,9 @@
       <c r="N10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="3"/>
+      <c r="O10" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
@@ -6594,7 +6938,9 @@
       <c r="N11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O11" s="3"/>
+      <c r="O11" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
@@ -6643,7 +6989,9 @@
       <c r="N12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O12" s="3"/>
+      <c r="O12" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
@@ -6692,7 +7040,9 @@
       <c r="N13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="3"/>
+      <c r="O13" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
@@ -6741,7 +7091,9 @@
       <c r="N14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="3"/>
+      <c r="O14" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
@@ -6790,7 +7142,9 @@
       <c r="N15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O15" s="3"/>
+      <c r="O15" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
@@ -6839,7 +7193,9 @@
       <c r="N16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O16" s="3"/>
+      <c r="O16" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
@@ -6888,7 +7244,9 @@
       <c r="N17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O17" s="3"/>
+      <c r="O17" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
@@ -6937,7 +7295,9 @@
       <c r="N18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O18" s="3"/>
+      <c r="O18" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
@@ -6986,7 +7346,9 @@
       <c r="N19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O19" s="3"/>
+      <c r="O19" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
@@ -7035,7 +7397,9 @@
       <c r="N20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O20" s="3"/>
+      <c r="O20" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
@@ -7047,13 +7411,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
       <formula>"="</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
       <formula>"+"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7880,13 +8244,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"="</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"+"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8464,13 +8828,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:XFD21 A2:I21 A22:XFD1048576">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>"="</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"+"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8483,16 +8847,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3729BD-F75F-DA40-A394-F4274E14071C}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A10" zoomScale="131" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="10.83203125" style="4"/>
+    <col min="3" max="5" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="13" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -8513,7 +8877,9 @@
       <c r="D2" s="6">
         <v>45705</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="6">
+        <v>45712</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -8534,7 +8900,9 @@
       <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -8555,7 +8923,9 @@
       <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -8576,7 +8946,9 @@
       <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -8597,7 +8969,9 @@
       <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -8618,7 +8992,9 @@
       <c r="D7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -8639,7 +9015,9 @@
       <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -8660,7 +9038,9 @@
       <c r="D9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -8681,7 +9061,9 @@
       <c r="D10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -8702,7 +9084,9 @@
       <c r="D11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -8723,7 +9107,9 @@
       <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -8744,7 +9130,9 @@
       <c r="D13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -8765,7 +9153,9 @@
       <c r="D14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -8786,7 +9176,9 @@
       <c r="D15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -8807,7 +9199,9 @@
       <c r="D16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -8828,7 +9222,9 @@
       <c r="D17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -8849,7 +9245,9 @@
       <c r="D18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -8870,7 +9268,9 @@
       <c r="D19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -8891,7 +9291,9 @@
       <c r="D20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -8912,7 +9314,9 @@
       <c r="D21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -8933,7 +9337,9 @@
       <c r="D22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -8954,7 +9360,9 @@
       <c r="D23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -8975,7 +9383,9 @@
       <c r="D24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -8996,7 +9406,9 @@
       <c r="D25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -9017,7 +9429,9 @@
       <c r="D26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="3"/>
+      <c r="E26" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -9038,7 +9452,9 @@
       <c r="D27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="3"/>
+      <c r="E27" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -9059,7 +9475,9 @@
       <c r="D28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="3"/>
+      <c r="E28" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -9080,7 +9498,9 @@
       <c r="D29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -9101,7 +9521,9 @@
       <c r="D30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -9122,7 +9544,9 @@
       <c r="D31" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -9143,7 +9567,9 @@
       <c r="D32" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="3"/>
+      <c r="E32" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -9164,7 +9590,9 @@
       <c r="D33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="3"/>
+      <c r="E33" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -9185,7 +9613,9 @@
       <c r="D34" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E34" s="3"/>
+      <c r="E34" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -9206,7 +9636,9 @@
       <c r="D35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E35" s="3"/>
+      <c r="E35" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -9219,24 +9651,24 @@
     <sortCondition ref="B3:B34"/>
   </sortState>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"="</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
       <formula>"+"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"="</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"+"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9682,10 +10114,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"+"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9698,15 +10130,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C3BA65-1DA3-D742-AE85-09580D9484E5}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView zoomScale="132" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -9724,7 +10156,9 @@
       <c r="C2" s="17">
         <v>45703</v>
       </c>
-      <c r="D2" s="15"/>
+      <c r="D2" s="17">
+        <v>45710</v>
+      </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -9742,7 +10176,9 @@
       <c r="C3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -9760,7 +10196,9 @@
       <c r="C4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -9778,7 +10216,9 @@
       <c r="C5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="15"/>
+      <c r="D5" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
@@ -9796,7 +10236,9 @@
       <c r="C6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="15"/>
+      <c r="D6" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
@@ -9814,7 +10256,9 @@
       <c r="C7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="15"/>
+      <c r="D7" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
@@ -9832,7 +10276,9 @@
       <c r="C8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="15"/>
+      <c r="D8" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
@@ -9850,7 +10296,9 @@
       <c r="C9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="15"/>
+      <c r="D9" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
@@ -9868,7 +10316,9 @@
       <c r="C10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="15"/>
+      <c r="D10" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
@@ -9886,7 +10336,9 @@
       <c r="C11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="15"/>
+      <c r="D11" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
@@ -9904,7 +10356,9 @@
       <c r="C12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="15"/>
+      <c r="D12" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
@@ -9922,7 +10376,9 @@
       <c r="C13" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="15"/>
+      <c r="D13" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
@@ -9940,7 +10396,9 @@
       <c r="C14" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
@@ -9958,7 +10416,9 @@
       <c r="C15" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="15"/>
+      <c r="D15" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
@@ -9976,7 +10436,9 @@
       <c r="C16" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="15"/>
+      <c r="D16" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
@@ -9994,7 +10456,9 @@
       <c r="C17" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="15"/>
+      <c r="D17" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
@@ -10012,7 +10476,9 @@
       <c r="C18" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="15"/>
+      <c r="D18" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
@@ -10030,7 +10496,9 @@
       <c r="C19" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="15"/>
+      <c r="D19" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
@@ -10048,7 +10516,9 @@
       <c r="C20" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="15"/>
+      <c r="D20" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
@@ -10066,7 +10536,9 @@
       <c r="C21" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="15"/>
+      <c r="D21" s="18" t="s">
+        <v>18</v>
+      </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
@@ -10079,13 +10551,13 @@
     <sortCondition ref="B21"/>
   </sortState>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"="</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"+"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>